<commit_message>
skill mismatch model 2.0
</commit_message>
<xml_diff>
--- a/skill by sector.xlsx
+++ b/skill by sector.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angzhinuo/Desktop/datathon/datathon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1D9521-99B5-B946-BC7D-CE1DE4F6E142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEEF4C2D-726F-7942-ACA1-BBA0F8252FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10280" yWindow="600" windowWidth="20740" windowHeight="17040" xr2:uid="{4A994717-86C2-1D44-89C3-FB8A60DDF68C}"/>
+    <workbookView xWindow="12080" yWindow="460" windowWidth="17700" windowHeight="17040" activeTab="1" xr2:uid="{4A994717-86C2-1D44-89C3-FB8A60DDF68C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>civil engineers</t>
   </si>
@@ -44,9 +45,6 @@
     <t>skills</t>
   </si>
   <si>
-    <t>Able to speak English,bahasa Malaysia, mandarin, cost counting to capture company’costs of production, autoCAD, planning and forethought,communication effective to superiors, college.leadership in research and practical, problem solving using generic and ad hoc method.nalysis information and make decision, project management in initiating,planing, executing, controlling and closing the work. Contruction management , quality management.failute analysis. Schematic design, Microsoft projects, technical analysis, forecasting price, market</t>
-  </si>
-  <si>
     <t>Carrying out maintenance and upgrading of all buildings and public facilities and supervising engineering related issues;Advising on and designing structures such as bridges, dams, docks, roads, airports, railways, pipelines, waste disposal and flood control systems, and industrial and other large buildings;Determining and specifying construction methods, materials and quality standards, and directing construction work;Establishing control systems to ensure efficient functioning of structures as well as safety and environmental protection;Organising and directing site labour and the delivery of construction materials, plant and equipment needed for construction projects;Administering contracts and verifying and certifying the satisfactory completion of construction;Studying and advising on technological aspects of particular materials/processes or systems related to civil engineering work;Quantity surveying of plans for bid, contract, contract assessment and other related tasks;Maintaining technical liaison and consultancy with other relevant specialists;supervising the testing and commissioning of completed work;andEnhancing knowledge and coordinating work performance</t>
   </si>
   <si>
@@ -56,9 +54,6 @@
     <t>Preparing and delivering lessons to students on fundamental topics in music;Organising performance groups and directing their rehearsals;Planning and preparing lessons in accordance with the prescribed/ recommended curriculum;Teaching and supervising students’ class work and discipline;Preparing, assigning and marking exercises, assignments and tests to evaluate student progress;Preparing reports on students’ work and conferring with other teachers and parents;Participating in staff meetings and educational conferences and workshops;Organising or assisting in co-curricular activities;Performing related tasks; andEnhancing knowledge and coordinating work performance</t>
   </si>
   <si>
-    <t>Speak English,bahasa Malaysia,mandarin, writing and expressing business messages effectively In written form, planning drafting and revising, singing, lesson planning, communication,curriculum design,listening,microsoft office, leadership, performance management, problem solving, speaking</t>
-  </si>
-  <si>
     <t>job description</t>
   </si>
   <si>
@@ -71,7 +66,85 @@
     <t>Preparing and delivering lessons to students on fundamental topics in arts;Explaining and demonstrating artistic techniques;Planning and preparing lessons in accordance with the prescribed/recommended curriculum;Teaching and supervising students’ class work and discipline;Preparing, assigning and marking exercises, assignments and tests to evaluate student progress;Preparing reports on students’ work and conferring with other teachers and parents;Participating in staff meetings and educational conferences and workshops;Organising or assisting in co-curricular activities;Performing related tasks; and Enhancing knowledge and coordinating work performance.</t>
   </si>
   <si>
-    <t>English,malaysia,mandarin,communication,leadership,painting,speaking,lesson planning</t>
+    <t>Able to speak English,bahasa Malaysia, mandarin, cost counting to capture company’costs of production, autoCAD, planning and forethought,communication effective to superiors &amp; college,leadership in research and practical, problem solving using generic and ad hoc method,analysis information and make decision, project management in initiating,planing, executing, controlling and closing the work. Contruction management , quality management,failute analysis. Schematic design, Microsoft projects, technical analysis, forecasting price &amp; market</t>
+  </si>
+  <si>
+    <t>primary school teacher</t>
+  </si>
+  <si>
+    <t>Being responsible for the curriculum, co-curriculum, student affairs management, office management and administration;Preparing teaching programmes such as reading, writing and arithmetic according to the prescribed or recommended curriculum;Preparing, supervising and marking tests, projects and assignments to train pupils and to evaluate their progress, and giving additional guidance if necessary;Organising and supervising pupils’ co-curricular activities such as assisting in sports activities, school concert, visits and special programmes;Encouraging the personal development of pupils and discussing their progress with parents;Maintaining attendance records and school discipline;Participating in staff meetings and educational conferences and workshops;Performing related tasks;Enhancing knowledge and coordinating work performance.</t>
+  </si>
+  <si>
+    <t>vocational teacher</t>
+  </si>
+  <si>
+    <t>Planning and preparing lessons in accordance with the prescribed/ recommended curriculum;Teaching and supervising students class work and discipline;Preparing, assigning and marking exercises, assignments and tests to evaluate student progress;Preparing reports on students’ work and conferring with other teachers and parents;Participating in staff meetings and educational conferences and workshops;Organising or assisting in co-curricular activities;Performing related tasks;enhancing knowledge and coordinating work performance</t>
+  </si>
+  <si>
+    <t>korean language teacher</t>
+  </si>
+  <si>
+    <t>Coordinating all language programme activities including selecting participants, teaching, assessing course participants, as well as conducting studies and research for training requirements;Planning, preparing and delivering lessons according to classes and age groups;Marking and giving appropriate feedback on oral and written work;Formulating and writing new materials;Participating in social and cultural activities;Carrying out freelance teaching on a one-to-one basis;Conducting specialist courses for adults or business people who may require knowledge of scientific, technical or commercial terms;Performing related tasks;Enhancing knowledge and coordinating work performance.</t>
+  </si>
+  <si>
+    <t>Speak English,bahasa Malaysia,mandarin, writing and expressing business messages effectively In written form, planning drafting and revising, singing, lesson planning, communication,curriculum design,listening,microsoft office, leadership, performance management, problem solving, speaking,teaching</t>
+  </si>
+  <si>
+    <t>English,malaysia,mandarin,communication,leadership,painting,speaking,lesson planning,teaching</t>
+  </si>
+  <si>
+    <t>Communication,mandarin,malay,english,speaking,writing,planning,listening,nursing,leadership,microsoft office,problem solving,patient,teaching</t>
+  </si>
+  <si>
+    <t>malay,chinese,english,illustration,graphic design,public speaking,speaking,mathematics,electronics,automation,teaching</t>
+  </si>
+  <si>
+    <t>mandarin,english,malay,korean,leadership,communication,speaking,microsoft office,public speaking,teaching</t>
+  </si>
+  <si>
+    <t>qualification</t>
+  </si>
+  <si>
+    <t>waiter</t>
+  </si>
+  <si>
+    <t>Setting tables with clean linen, cutlery, crockery and glassware;Setting and arranging tables and escorting guests to their tables;Presenting the menu and recommending menu items to customers;Taking orders and serving food and beverages;Serving food and beverages to customers;Presenting bills to customers and accepting payment;Cleaning the dining area;Performing related tasks.</t>
+  </si>
+  <si>
+    <t>source of data:</t>
+  </si>
+  <si>
+    <t>chef</t>
+  </si>
+  <si>
+    <t>Planning meals and menus, ordering food supplies and preparing and cooking food;Monitoring food quality;Demonstrating techniques and advising on cooking procedures;Planning, supervising and coordinating work in the kitchen;Ensuring cleanliness of crockery, utensils, kitchen equipment and work areas;Organising food promotions;Determining dry and wet ingredients for cooking, receiving and checking ingredients, preparing ingredients, preserving the cleanliness of equipment and kitchen area, and ensuring that kitchenware is stored and locked;Ensuring safe and sanitary food handling practices are complied with;Performing related tasks;Supervising other workers.</t>
+  </si>
+  <si>
+    <t>leadership,inventory management,meal preparation,cook,planning,smell,taste,quality management,team management,written communication,weighing,cutting skills,culinary arts,creativity,food safety,nutrition,multitasking</t>
+  </si>
+  <si>
+    <t>communication,food preparation,speaking,listening,active listening,bartending,time management,writing,meal serving,note taking,good memory,excellent verbal,accept critism</t>
+  </si>
+  <si>
+    <t>university and higher education teaching professionals</t>
+  </si>
+  <si>
+    <t>Delivering lectures and conducting tutorials, research and releasing publications;Giving lectures, supervising thesis projects, managing practical work/tutorials and preparing lecture notes/laboratory manuals;Conducting examination matters, monitoring the practical training of students, assisting in reviewing / preparing the curriculum / syllabus, engaging in research work and undertaking student development work;Providing consultancy services to students and outsiders, supervising projects, theses and student papers, conducting research, publishing journals, articles, books and other forms of related publications, services, performing community and professional services, helping students develop their potential and character, and managing academic-related activities;Designing and modifying the curricula and preparing courses of study in accordance with the requirements;Encouraging discussion and independent thinking among students;Conducting research and developing concepts, theories and operational methods for application in the industry and other fields;Assisting in co-curricular activities;Performing related tasks;Enhancing knowledge and coordinating work performance.</t>
+  </si>
+  <si>
+    <t>english,research,marketing,communication,planning,leadership,malay,teaching,microsoft office,writing,graphic design,programming,speaking,business management,critical thinking,collaborating,</t>
+  </si>
+  <si>
+    <t>administrative &amp; executive secretary</t>
+  </si>
+  <si>
+    <t>Drafting correspondence and minutes;Obtaining, proposing and monitoring deadlines and follow-up dates;Screening requests for meetings, scheduling and organising meetings and travel arrangements for the head of unit and other members of staff;Assisting in the preparation of budgets, monitoring of expenditures, drafting of contracts and purchase or taking of orders;Assisting the head of unit and other staff with queries of an administrative or organisational nature;Liaising with other staff about a range of matters relating to organisational operations;Writing and answering business or technical letters and other similar correspondence;Performing related tasks;Supervising, scheduling and monitoring the tasks of other workers.</t>
+  </si>
+  <si>
+    <t>english,mandarin,malay,communication,filling,scheduling,microsoft office,computer literacy,administrative management,record keeping,business writing,calendar management,corporate communications,proofreading,file management,secretarial,corporate reporting,document management,cash flow analysis,</t>
+  </si>
+  <si>
+    <t>https://www.ilmia.gov.my/bda-myjobprofile/</t>
   </si>
 </sst>
 </file>
@@ -445,114 +518,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240730E0-74C6-DB44-8CBF-6568E3D2B4CC}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="B22" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14452077-E62B-3145-83E0-FB9E6346E274}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="2:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="2:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="2:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="2:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="2:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="2:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="B22" s="1"/>
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>